<commit_message>
Added source of datasets to top of exploration notebooks
</commit_message>
<xml_diff>
--- a/datasets/Australian Energy Statistics 2023 Table O_0(1).xlsx
+++ b/datasets/Australian Energy Statistics 2023 Table O_0(1).xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{379E4880-F197-46AA-BC51-D57CDA5FA8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF313A7F-F695-4C3F-B2C5-805304165EBB}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="17280" windowHeight="12336" tabRatio="821" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1944" yWindow="1500" windowWidth="17280" windowHeight="8880" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Title page" sheetId="12" r:id="rId1"/>
@@ -2871,8 +2871,8 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -14041,7 +14041,7 @@
   </sheetPr>
   <dimension ref="A1:AJ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="N15" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K36" sqref="K36"/>
       <selection pane="topRight" activeCell="K36" sqref="K36"/>

</xml_diff>